<commit_message>
Week 1 - flutter learning - Anushka Chincholkar
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anushka Chincholkar.LAPTOP-PVP8F6JH\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC22099-0326-4C99-B5B0-17D951FECB4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Team Members</t>
   </si>
@@ -46,13 +52,16 @@
   </si>
   <si>
     <t xml:space="preserve"> Work Done Upto</t>
+  </si>
+  <si>
+    <t>Studied basic concepts of Flutter toolkit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +101,24 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -148,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,9 +197,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,6 +249,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,31 +442,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
         <v>44234</v>
       </c>
@@ -427,42 +480,45 @@
         <v>44255</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -477,24 +533,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated progress upto 7th February
Studied basic concepts of flutter development
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anushka Chincholkar.LAPTOP-PVP8F6JH\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7D8796-087E-410B-8073-27E67A952502}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Team Members</t>
   </si>
@@ -49,13 +55,16 @@
   </si>
   <si>
     <t>Setup flutter environment and learned basics of dart</t>
+  </si>
+  <si>
+    <t>Studied basic concepts of development in flutter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +114,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -151,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,9 +200,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,6 +252,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,20 +445,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -416,7 +469,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
         <v>44234</v>
       </c>
@@ -430,7 +483,7 @@
         <v>44255</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -438,37 +491,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -483,24 +539,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
progress report update by tejomay
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\trail\Racket-Shuttle_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655C5C7E-4A9E-4321-9EF4-07B9A35B3E3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Team Members</t>
   </si>
@@ -64,12 +63,15 @@
   </si>
   <si>
     <t>studied basics of dart and setup of flutter env</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flutter environment setup in android studio, started learning dart basics </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,23 +209,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -259,23 +244,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,17 +419,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="58.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -518,6 +486,9 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -551,7 +522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -563,7 +534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Progress report updated by Suruchi
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\trail\Racket-Shuttle_Tracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Team Members</t>
   </si>
@@ -66,13 +61,16 @@
   </si>
   <si>
     <t xml:space="preserve">Flutter environment setup in android studio, started learning dart basics </t>
+  </si>
+  <si>
+    <t>Set up flutter environment and studied basics of dart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,10 +206,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,7 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,20 +415,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="58.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -443,7 +439,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="B2" s="1">
         <v>44234</v>
       </c>
@@ -457,7 +453,7 @@
         <v>44255</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -465,7 +461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -473,17 +469,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -491,12 +487,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -504,7 +503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -522,24 +521,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Shreya Sahni commit for Feb 1st week
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya Sahni\AndroidStudioProjects\SoftLab\Racket-Shuttle_Tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB310BC-B45B-488B-A947-8D184801CEE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Team Members</t>
   </si>
@@ -64,13 +70,16 @@
   </si>
   <si>
     <t>Set up flutter environment and studied basics of dart</t>
+  </si>
+  <si>
+    <t>1. Studied syntax and other basics of dart, flutter 2. Set up flutter plugin with android studio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +215,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +267,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,20 +460,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="58.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="58.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -439,7 +484,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>44234</v>
       </c>
@@ -453,7 +498,7 @@
         <v>44255</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -461,7 +506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -469,17 +514,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -487,7 +535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -495,7 +543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -503,7 +551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -521,24 +569,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Work done over preceding week
Created basic app in flutter
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,32 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\trail\Racket-Shuttle_Tracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Team Members</t>
   </si>
@@ -40,12 +27,18 @@
     <t>Setup flutter environment and learned basics of dart</t>
   </si>
   <si>
+    <t>Learned how to use layouts and widgets of Flutter</t>
+  </si>
+  <si>
     <t>Anushka Chincholkar</t>
   </si>
   <si>
     <t>Studied basic concepts of development in flutter</t>
   </si>
   <si>
+    <t>Developed basic app with flutter widgets and layouts</t>
+  </si>
+  <si>
     <t>Atharva Kulkarni</t>
   </si>
   <si>
@@ -64,110 +57,106 @@
     <t xml:space="preserve">Flutter environment setup in android studio, started learning dart basics </t>
   </si>
   <si>
+    <t>Learnt how to incorporate images and custom fonts inside our flutter app, also tested out hot reload in flutter</t>
+  </si>
+  <si>
     <t>Suruchi Shrey</t>
   </si>
   <si>
     <t>Set up flutter environment and studied basics of dart</t>
   </si>
   <si>
+    <t>Made a basic app, learned using widgets and some gestures of flutter</t>
+  </si>
+  <si>
     <t>Pradnya Kore</t>
   </si>
   <si>
     <t>studied basics of dart and setup of flutter env</t>
   </si>
   <si>
+    <t>Learned how to work with widgets and other functionalities of Flutter</t>
+  </si>
+  <si>
     <t>Sanskruti Nakhale</t>
   </si>
   <si>
     <t>Learned Basics of Flutter and Dart</t>
-  </si>
-  <si>
-    <t>Learned how to use layouts and widgets of Flutter</t>
-  </si>
-  <si>
-    <t>Made a basic app, learned using widgets and some gestures of flutter</t>
-  </si>
-  <si>
-    <t>Learned how to work with widgets and other functionalities of Flutter</t>
-  </si>
-  <si>
-    <t>Learnt how to incorporate images and custom fonts inside our flutter app, also tested out hot reload in flutter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -325,7 +314,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln cap="flat" cmpd="sng" w="9525" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -334,13 +323,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln cap="flat" cmpd="sng" w="25400" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln cap="flat" cmpd="sng" w="38100" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -350,7 +339,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="20000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -359,7 +348,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -368,7 +357,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -378,12 +367,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -414,7 +403,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -433,7 +422,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -445,46 +434,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="76" customWidth="1"/>
-    <col min="3" max="3" width="84" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="17.86"/>
+    <col customWidth="1" min="2" max="2" width="76.0"/>
+    <col customWidth="1" min="3" max="3" width="84.0"/>
+    <col customWidth="1" min="4" max="11" width="8.43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="2">
-        <v>44234</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44241</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44248</v>
-      </c>
-      <c r="E2" s="2">
-        <v>44255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="B2" s="3">
+        <v>44234.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44241.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44248.0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44255.0</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -492,105 +479,416 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="11" width="8.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" customHeight="1"/>
+    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="3" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="11" width="8.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" customHeight="1"/>
+    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="3" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Shreya update for week 2
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya Sahni\AndroidStudioProjects\SoftLab\Racket-Shuttle_Tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875017C-AD1E-4A20-9832-498B8C01209D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Team Members</t>
   </si>
@@ -82,81 +91,87 @@
   </si>
   <si>
     <t>Learned Basics of Flutter and Dart</t>
+  </si>
+  <si>
+    <t>Continued learning and practising Dart, Flutter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -314,7 +329,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" w="9525" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -323,13 +338,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="25400" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="38100" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -339,7 +354,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="20000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -348,7 +363,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -357,7 +372,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -367,12 +382,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -403,7 +418,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -422,7 +437,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -434,44 +449,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="2" max="2" width="76.0"/>
-    <col customWidth="1" min="3" max="3" width="84.0"/>
-    <col customWidth="1" min="4" max="11" width="8.43"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="76" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="4" max="11" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="B2" s="3">
-        <v>44234.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>44241.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44248.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>44255.0</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="B2" s="2">
+        <v>44234</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44241</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44248</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44255</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -482,18 +500,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -501,15 +519,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -520,7 +541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -531,7 +552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:5" ht="14.25" customHeight="1">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -542,7 +563,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:5" ht="14.25" customHeight="1">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -550,12 +571,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -644,24 +665,20 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="11" width="8.43"/>
+    <col min="1" max="11" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -765,24 +782,20 @@
     <row r="99" ht="14.25" customHeight="1"/>
     <row r="100" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="11" width="8.43"/>
+    <col min="1" max="11" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -886,9 +899,7 @@
     <row r="99" ht="14.25" customHeight="1"/>
     <row r="100" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Shreya update for week 3
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,21 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya Sahni\AndroidStudioProjects\SoftLab\Racket-Shuttle_Tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F208183D-1363-4415-AE29-5291544D6317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>Team Members</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Work Done Upto</t>
+  </si>
+  <si>
+    <t>7-Feb</t>
+  </si>
+  <si>
+    <t>14-Feb</t>
+  </si>
+  <si>
+    <t>21-Feb</t>
+  </si>
+  <si>
+    <t>28-Feb</t>
+  </si>
+  <si>
+    <t>Sanchita Kasat</t>
+  </si>
+  <si>
+    <t>Setup flutter environment and learned basics of dart</t>
+  </si>
+  <si>
+    <t>Learned how to use layouts and widgets of Flutter</t>
+  </si>
+  <si>
+    <t>Anushka Chincholkar</t>
+  </si>
+  <si>
+    <t>Studied basic concepts of development in flutter</t>
+  </si>
+  <si>
+    <t>Developed basic app with flutter widgets and layouts</t>
+  </si>
+  <si>
+    <t>Atharva Kulkarni</t>
+  </si>
+  <si>
+    <t>Studied basics of dart and flashed LineageOS on old android smartphone for testing purposes</t>
+  </si>
+  <si>
+    <t>Shreya Sahni</t>
+  </si>
+  <si>
+    <t>1. Studied syntax and other basics of dart, flutter 2. Set up flutter plugin with android studio</t>
+  </si>
+  <si>
+    <t>Continued learning and practising Dart, Flutter</t>
+  </si>
+  <si>
+    <t>Tejomay Padole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flutter environment setup in android studio, started learning dart basics </t>
+  </si>
+  <si>
+    <t>Learnt how to incorporate images and custom fonts inside our flutter app, also tested out hot reload in flutter</t>
+  </si>
+  <si>
+    <t>Suruchi Shrey</t>
+  </si>
+  <si>
+    <t>Set up flutter environment and studied basics of dart</t>
+  </si>
+  <si>
+    <t>Made a basic app, learned using widgets and some gestures of flutter</t>
+  </si>
+  <si>
+    <t>Pradnya Kore</t>
+  </si>
+  <si>
+    <t>studied basics of dart and setup of flutter env</t>
+  </si>
+  <si>
+    <t>Learned how to work with widgets and other functionalities of Flutter</t>
+  </si>
+  <si>
+    <t>Sanskruti Nakhale</t>
+  </si>
+  <si>
+    <t>Learned Basics of Flutter and Dart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flutter Learning Continued and Applying to make a basic app </t>
+  </si>
+  <si>
+    <t>Explored Firebase and learned how to integrate it with a Flutter application</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,6 +155,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -376,148 +487,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.796875" customWidth="1"/>
+    <col min="2" max="2" width="26.296875" customWidth="1"/>
+    <col min="3" max="3" width="26.69921875" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="26.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Team Members</v>
-      </c>
-      <c r="B1" t="str">
-        <v xml:space="preserve"> Work Done Upto</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="str">
-        <v>7-Feb</v>
-      </c>
-      <c r="C2" t="str">
-        <v>14-Feb</v>
-      </c>
-      <c r="D2" t="str">
-        <v>21-Feb</v>
-      </c>
-      <c r="E2" t="str">
-        <v>28-Feb</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Sanchita Kasat</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Setup flutter environment and learned basics of dart</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Learned how to use layouts and widgets of Flutter</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Anushka Chincholkar</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Studied basic concepts of development in flutter</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Developed basic app with flutter widgets and layouts</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Atharva Kulkarni</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Studied basics of dart and flashed LineageOS on old android smartphone for testing purposes</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Shreya Sahni</v>
-      </c>
-      <c r="B6" t="str">
-        <v>1. Studied syntax and other basics of dart, flutter 2. Set up flutter plugin with android studio</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Continued learning and practising Dart, Flutter</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Tejomay Padole</v>
-      </c>
-      <c r="B7" t="str">
-        <v xml:space="preserve">Flutter environment setup in android studio, started learning dart basics </v>
-      </c>
-      <c r="C7" t="str">
-        <v>Learnt how to incorporate images and custom fonts inside our flutter app, also tested out hot reload in flutter</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Suruchi Shrey</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Set up flutter environment and studied basics of dart</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Made a basic app, learned using widgets and some gestures of flutter</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Pradnya Kore</v>
-      </c>
-      <c r="B9" t="str">
-        <v>studied basics of dart and setup of flutter env</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Learned how to work with widgets and other functionalities of Flutter</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Sanskruti Nakhale</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Learned Basics of Flutter and Dart</v>
-      </c>
-      <c r="C10" t="str">
-        <v xml:space="preserve">Flutter Learning Continued and Applying to make a basic app </v>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E10"/>
+    <ignoredError sqref="A1:E5 A7:E10 A6:C6 E6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sanchita week 3 update
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya Sahni\AndroidStudioProjects\SoftLab\Racket-Shuttle_Tracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F208183D-1363-4415-AE29-5291544D6317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Team Members</t>
   </si>
@@ -112,13 +106,16 @@
   </si>
   <si>
     <t>Explored Firebase and learned how to integrate it with a Flutter application</t>
+  </si>
+  <si>
+    <t>Integrating Google Maps API with Flutter geocoding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -487,14 +484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="16.796875" customWidth="1"/>
     <col min="2" max="2" width="26.296875" customWidth="1"/>
@@ -503,7 +500,7 @@
     <col min="5" max="5" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -525,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30.6" customHeight="1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -535,8 +532,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32.4" customHeight="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -547,7 +547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="29.4" customHeight="1">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -555,7 +555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="31.2" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -569,7 +569,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" customHeight="1">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -580,7 +580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="29.4" customHeight="1">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -591,7 +591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="32.4" customHeight="1">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -602,7 +602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="31.2" customHeight="1">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -616,18 +616,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E5 A7:E10 A6:C6 E6" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E2 A7:E10 A6:C6 E6 A4:E5 A3:C3 E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -637,12 +637,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Week 3 Progress report
</commit_message>
<xml_diff>
--- a/Progress_report.xlsx
+++ b/Progress_report.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anushka Chincholkar.LAPTOP-PVP8F6JH\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8602B6BC-B735-424D-BBF8-0BFA0C58EA97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Team Members</t>
   </si>
@@ -115,13 +121,16 @@
   </si>
   <si>
     <t>Studied firebase and how to use it with flutter</t>
+  </si>
+  <si>
+    <t>Studied basics of Flutter UI Design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -490,23 +499,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.75" customWidth="1"/>
     <col min="2" max="2" width="26.25" customWidth="1"/>
     <col min="3" max="3" width="26.75" customWidth="1"/>
-    <col min="4" max="4" width="66.875" customWidth="1"/>
+    <col min="4" max="4" width="66.83203125" customWidth="1"/>
     <col min="5" max="5" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -528,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.6" customHeight="1">
+    <row r="3" spans="1:5" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -542,7 +551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32.450000000000003" customHeight="1">
+    <row r="4" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -552,8 +561,11 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.45" customHeight="1">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -561,7 +573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.15" customHeight="1">
+    <row r="6" spans="1:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -575,7 +587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -589,7 +601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.45" customHeight="1">
+    <row r="8" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -603,7 +615,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32.450000000000003" customHeight="1">
+    <row r="9" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -614,7 +626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.15" customHeight="1">
+    <row r="10" spans="1:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -628,18 +640,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E2 A9:E9 A6:C6 E6 A4:E5 A3:C3 E3 A10:C10 E10 A7:C7 A8:C8 E8" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E2 A9:E9 A6:C6 E6 A5:E5 A3:C3 E3 A10:C10 E10 A7:C7 A8:C8 E8 A4:C4 E4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -649,12 +661,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>